<commit_message>
aligns search functionality with wikidata app
</commit_message>
<xml_diff>
--- a/data/translations.03_buehler.xlsx
+++ b/data/translations.03_buehler.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="42">
   <si>
     <t xml:space="preserve">key</t>
   </si>
@@ -52,6 +52,9 @@
     <t xml:space="preserve">Im Suchschlitz können der Name oder die Wikidata-Entitätsnummer (z. B. Q1234) eingegeben werden. Um zwei zusammengehörige Begriffe (meist Vor‑ und Nachname) zu suchen, ist ein »+« zwischen dem ersten und dem zweiten Begriff anzugeben (Beispiel: Dieterle +Marie).</t>
   </si>
   <si>
+    <t xml:space="preserve">On peut indiquer dans la barre de recherche le nom ou l’identifiant d’entité Wikidata (par ex. Q1234). Pour rechercher deux termes associés (le plus souvent prénom et nom), il faut indiquer un « + » entre le premier et le deuxième terme (ex. Marie+Dieterle)</t>
+  </si>
+  <si>
     <t xml:space="preserve">show_order</t>
   </si>
   <si>
@@ -109,47 +112,13 @@
     <t xml:space="preserve">send_as_mail</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">als Email versenden an </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">bibliothek@dfk-paris.org</t>
-    </r>
+    <t xml:space="preserve">als Email versenden an bibliothek@dfk-paris.org</t>
   </si>
   <si>
     <t xml:space="preserve">envoyer à bibliothek@dfk-paris.org</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">send as email to </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">bibliothek@dfk-paris.org</t>
-    </r>
+    <t xml:space="preserve">send as email to bibliothek@dfk-paris.org</t>
   </si>
   <si>
     <t xml:space="preserve">order</t>
@@ -213,6 +182,7 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -257,13 +227,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -398,7 +372,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.71484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -406,7 +380,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.18"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="34.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="34.97"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1021" min="5" style="1" width="30.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1022" style="1" width="11.57"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1025" style="1" width="30.71"/>
@@ -447,131 +421,134 @@
       <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="C9" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D9" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -703,8 +680,8 @@
     <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B9" r:id="rId1" display="bibliothek@dfk-paris.org"/>
-    <hyperlink ref="D9" r:id="rId2" display="bibliothek@dfk-paris.org"/>
+    <hyperlink ref="B9" r:id="rId1" display="als Email versenden an bibliothek@dfk-paris.org"/>
+    <hyperlink ref="D9" r:id="rId2" display="send as email to bibliothek@dfk-paris.org"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>